<commit_message>
update adcore template files
</commit_message>
<xml_diff>
--- a/adcore/2018/templates/2018-brand-long.xlsx
+++ b/adcore/2018/templates/2018-brand-long.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyedmonds/Dropbox/git/repo/agency/adcore/2018/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAF31124-4976-B44C-A125-A8248168AEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FD0329-700A-AA43-AC43-882CE090E24A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3820" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CMS" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="606">
   <si>
     <t>Offer Code</t>
   </si>
@@ -1798,6 +1798,57 @@
   </si>
   <si>
     <t>WXX_XX_XXX_XXX16CL</t>
+  </si>
+  <si>
+    <t>Carousel</t>
+  </si>
+  <si>
+    <t>Section 1 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 2 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 3 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 4 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 5 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 6 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 7 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 8 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 9 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 10 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 11 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 12 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 13 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 14 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 15 Accordion/Custom List</t>
+  </si>
+  <si>
+    <t>Section 16 Accordion/Custom List</t>
   </si>
 </sst>
 </file>
@@ -1876,13 +1927,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97FD37EF-440B-164F-A671-9404BC5B49C2}" name="Table2" displayName="Table2" ref="A1:D170" totalsRowShown="0">
-  <autoFilter ref="A1:D170" xr:uid="{46B822AB-FF4E-B747-B408-B19D12290E92}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97FD37EF-440B-164F-A671-9404BC5B49C2}" name="Table2" displayName="Table2" ref="A1:E170" totalsRowShown="0">
+  <autoFilter ref="A1:E170" xr:uid="{46B822AB-FF4E-B747-B408-B19D12290E92}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{17C01559-4713-534F-9A9B-549B487B8F5A}" name="Module"/>
     <tableColumn id="2" xr3:uid="{FC851083-6D66-B24A-8460-C785CF4AAE2A}" name="Offer Code"/>
     <tableColumn id="3" xr3:uid="{DEC14A67-67A3-0F43-B97F-64C2002A3EBD}" name="Description"/>
     <tableColumn id="4" xr3:uid="{CDB8C82C-9162-FA42-B6A8-8BDC4B93A20B}" name="Blank"/>
+    <tableColumn id="5" xr3:uid="{E3D87CD0-A26D-B04F-9E3E-5755668D42BE}" name="Carousel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2209,21 +2261,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D170"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2236,8 +2289,11 @@
       <c r="D1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2248,7 +2304,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2262,7 +2318,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2276,7 +2332,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2287,7 +2343,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2298,7 +2354,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2309,7 +2365,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2320,7 +2376,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2331,7 +2387,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2342,7 +2398,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2353,7 +2409,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2364,7 +2420,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2375,7 +2431,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2386,7 +2442,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2397,7 +2453,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2408,7 +2464,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2419,7 +2475,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2430,7 +2486,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2441,7 +2497,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -2452,7 +2508,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2463,7 +2519,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2474,7 +2530,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2485,7 +2541,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -2493,13 +2549,16 @@
         <v>426</v>
       </c>
       <c r="C24" t="s">
-        <v>388</v>
+        <v>590</v>
       </c>
       <c r="D24" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2510,7 +2569,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2521,7 +2580,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2532,7 +2591,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2543,7 +2602,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -2554,7 +2613,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -2565,7 +2624,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -2576,7 +2635,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2587,7 +2646,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -2595,13 +2654,16 @@
         <v>435</v>
       </c>
       <c r="C33" t="s">
-        <v>389</v>
+        <v>591</v>
       </c>
       <c r="D33" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2612,7 +2674,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2623,7 +2685,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2634,7 +2696,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2645,7 +2707,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2656,7 +2718,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -2667,7 +2729,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -2678,7 +2740,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -2689,7 +2751,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -2697,13 +2759,16 @@
         <v>444</v>
       </c>
       <c r="C42" t="s">
-        <v>390</v>
+        <v>592</v>
       </c>
       <c r="D42" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -2714,7 +2779,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -2725,7 +2790,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -2736,7 +2801,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -2747,7 +2812,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -2758,7 +2823,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -2769,7 +2834,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -2780,7 +2845,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -2791,7 +2856,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -2799,13 +2864,16 @@
         <v>453</v>
       </c>
       <c r="C51" t="s">
-        <v>391</v>
+        <v>593</v>
       </c>
       <c r="D51" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -2816,7 +2884,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -2827,7 +2895,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -2838,7 +2906,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -2849,7 +2917,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -2860,7 +2928,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -2871,7 +2939,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -2882,7 +2950,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -2893,7 +2961,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>80</v>
       </c>
@@ -2901,13 +2969,16 @@
         <v>462</v>
       </c>
       <c r="C60" t="s">
-        <v>392</v>
+        <v>594</v>
       </c>
       <c r="D60" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>81</v>
       </c>
@@ -2918,7 +2989,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -2929,7 +3000,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>83</v>
       </c>
@@ -2940,7 +3011,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -2951,7 +3022,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -2962,7 +3033,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -2973,7 +3044,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>87</v>
       </c>
@@ -2984,7 +3055,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -2995,7 +3066,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>89</v>
       </c>
@@ -3003,13 +3074,16 @@
         <v>471</v>
       </c>
       <c r="C69" t="s">
-        <v>393</v>
+        <v>595</v>
       </c>
       <c r="D69" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -3020,7 +3094,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>91</v>
       </c>
@@ -3031,7 +3105,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>92</v>
       </c>
@@ -3042,7 +3116,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -3053,7 +3127,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>94</v>
       </c>
@@ -3064,7 +3138,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>95</v>
       </c>
@@ -3075,7 +3149,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -3086,7 +3160,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>97</v>
       </c>
@@ -3097,7 +3171,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -3105,13 +3179,16 @@
         <v>480</v>
       </c>
       <c r="C78" t="s">
-        <v>394</v>
+        <v>596</v>
       </c>
       <c r="D78" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>99</v>
       </c>
@@ -3122,7 +3199,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>100</v>
       </c>
@@ -3133,7 +3210,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>101</v>
       </c>
@@ -3144,7 +3221,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>102</v>
       </c>
@@ -3155,7 +3232,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>103</v>
       </c>
@@ -3166,7 +3243,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>104</v>
       </c>
@@ -3177,7 +3254,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>105</v>
       </c>
@@ -3188,7 +3265,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>106</v>
       </c>
@@ -3199,7 +3276,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>107</v>
       </c>
@@ -3207,13 +3284,16 @@
         <v>489</v>
       </c>
       <c r="C87" t="s">
-        <v>395</v>
+        <v>597</v>
       </c>
       <c r="D87" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>108</v>
       </c>
@@ -3224,7 +3304,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>109</v>
       </c>
@@ -3235,7 +3315,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>110</v>
       </c>
@@ -3246,7 +3326,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>111</v>
       </c>
@@ -3257,7 +3337,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>112</v>
       </c>
@@ -3268,7 +3348,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>113</v>
       </c>
@@ -3279,7 +3359,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>114</v>
       </c>
@@ -3290,7 +3370,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>115</v>
       </c>
@@ -3301,7 +3381,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>116</v>
       </c>
@@ -3309,13 +3389,16 @@
         <v>498</v>
       </c>
       <c r="C96" t="s">
-        <v>396</v>
+        <v>598</v>
       </c>
       <c r="D96" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>117</v>
       </c>
@@ -3326,7 +3409,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>118</v>
       </c>
@@ -3337,7 +3420,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>119</v>
       </c>
@@ -3348,7 +3431,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>120</v>
       </c>
@@ -3359,7 +3442,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>121</v>
       </c>
@@ -3370,7 +3453,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>122</v>
       </c>
@@ -3381,7 +3464,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>123</v>
       </c>
@@ -3392,7 +3475,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>124</v>
       </c>
@@ -3403,7 +3486,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>125</v>
       </c>
@@ -3411,13 +3494,16 @@
         <v>507</v>
       </c>
       <c r="C105" t="s">
-        <v>397</v>
+        <v>599</v>
       </c>
       <c r="D105" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>126</v>
       </c>
@@ -3428,7 +3514,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>127</v>
       </c>
@@ -3439,7 +3525,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>128</v>
       </c>
@@ -3450,7 +3536,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>129</v>
       </c>
@@ -3461,7 +3547,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>130</v>
       </c>
@@ -3472,7 +3558,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>131</v>
       </c>
@@ -3483,7 +3569,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>132</v>
       </c>
@@ -3494,7 +3580,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>133</v>
       </c>
@@ -3505,7 +3591,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>134</v>
       </c>
@@ -3513,13 +3599,16 @@
         <v>516</v>
       </c>
       <c r="C114" t="s">
-        <v>398</v>
+        <v>600</v>
       </c>
       <c r="D114" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>135</v>
       </c>
@@ -3530,7 +3619,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>136</v>
       </c>
@@ -3541,7 +3630,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>137</v>
       </c>
@@ -3552,7 +3641,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>138</v>
       </c>
@@ -3563,7 +3652,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>139</v>
       </c>
@@ -3574,7 +3663,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>140</v>
       </c>
@@ -3585,7 +3674,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>141</v>
       </c>
@@ -3596,7 +3685,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>142</v>
       </c>
@@ -3607,7 +3696,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>143</v>
       </c>
@@ -3615,13 +3704,16 @@
         <v>525</v>
       </c>
       <c r="C123" t="s">
-        <v>399</v>
+        <v>601</v>
       </c>
       <c r="D123" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>144</v>
       </c>
@@ -3632,7 +3724,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>145</v>
       </c>
@@ -3643,7 +3735,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>146</v>
       </c>
@@ -3654,7 +3746,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>147</v>
       </c>
@@ -3665,7 +3757,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>148</v>
       </c>
@@ -3676,7 +3768,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>149</v>
       </c>
@@ -3687,7 +3779,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>150</v>
       </c>
@@ -3698,7 +3790,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>151</v>
       </c>
@@ -3709,7 +3801,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>152</v>
       </c>
@@ -3717,13 +3809,16 @@
         <v>534</v>
       </c>
       <c r="C132" t="s">
-        <v>400</v>
+        <v>602</v>
       </c>
       <c r="D132" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>153</v>
       </c>
@@ -3734,7 +3829,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>154</v>
       </c>
@@ -3745,7 +3840,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>155</v>
       </c>
@@ -3756,7 +3851,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>156</v>
       </c>
@@ -3767,7 +3862,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>157</v>
       </c>
@@ -3778,7 +3873,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>158</v>
       </c>
@@ -3789,7 +3884,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>159</v>
       </c>
@@ -3800,7 +3895,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>160</v>
       </c>
@@ -3811,7 +3906,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>161</v>
       </c>
@@ -3819,13 +3914,16 @@
         <v>543</v>
       </c>
       <c r="C141" t="s">
-        <v>401</v>
+        <v>603</v>
       </c>
       <c r="D141" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E141" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>162</v>
       </c>
@@ -3836,7 +3934,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>163</v>
       </c>
@@ -3847,7 +3945,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>164</v>
       </c>
@@ -3858,7 +3956,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>165</v>
       </c>
@@ -3869,7 +3967,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>166</v>
       </c>
@@ -3880,7 +3978,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>167</v>
       </c>
@@ -3891,7 +3989,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>168</v>
       </c>
@@ -3902,7 +4000,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>169</v>
       </c>
@@ -3913,7 +4011,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>170</v>
       </c>
@@ -3921,13 +4019,16 @@
         <v>552</v>
       </c>
       <c r="C150" t="s">
-        <v>402</v>
+        <v>604</v>
       </c>
       <c r="D150" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E150" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>171</v>
       </c>
@@ -3938,7 +4039,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>172</v>
       </c>
@@ -3949,7 +4050,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>173</v>
       </c>
@@ -3960,7 +4061,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>174</v>
       </c>
@@ -3971,7 +4072,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>175</v>
       </c>
@@ -3982,7 +4083,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>176</v>
       </c>
@@ -3993,7 +4094,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>177</v>
       </c>
@@ -4004,7 +4105,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>178</v>
       </c>
@@ -4015,7 +4116,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>179</v>
       </c>
@@ -4023,13 +4124,16 @@
         <v>561</v>
       </c>
       <c r="C159" t="s">
-        <v>403</v>
+        <v>605</v>
       </c>
       <c r="D159" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E159" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>180</v>
       </c>
@@ -4163,8 +4267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4214,12 +4318,8 @@
       <c r="D2" t="s">
         <v>405</v>
       </c>
-      <c r="E2" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F2" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" t="s">
         <v>8</v>
       </c>
@@ -4237,12 +4337,8 @@
       <c r="D3" t="s">
         <v>406</v>
       </c>
-      <c r="E3" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F3" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" t="s">
         <v>233</v>
       </c>
@@ -4260,12 +4356,8 @@
       <c r="D4" t="s">
         <v>407</v>
       </c>
-      <c r="E4" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F4" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" t="s">
         <v>234</v>
       </c>
@@ -4283,12 +4375,8 @@
       <c r="D5" t="s">
         <v>408</v>
       </c>
-      <c r="E5" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F5" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" t="s">
         <v>10</v>
       </c>
@@ -4306,12 +4394,8 @@
       <c r="D6" t="s">
         <v>404</v>
       </c>
-      <c r="E6" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F6" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" t="s">
         <v>8</v>
       </c>
@@ -4329,12 +4413,8 @@
       <c r="D7" t="s">
         <v>409</v>
       </c>
-      <c r="E7" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F7" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" t="s">
         <v>236</v>
       </c>
@@ -4352,12 +4432,8 @@
       <c r="D8" t="s">
         <v>410</v>
       </c>
-      <c r="E8" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F8" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" t="s">
         <v>236</v>
       </c>
@@ -4375,12 +4451,8 @@
       <c r="D9" t="s">
         <v>411</v>
       </c>
-      <c r="E9" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F9" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" t="s">
         <v>236</v>
       </c>
@@ -4398,12 +4470,8 @@
       <c r="D10" t="s">
         <v>412</v>
       </c>
-      <c r="E10" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F10" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" t="s">
         <v>236</v>
       </c>
@@ -4421,12 +4489,8 @@
       <c r="D11" t="s">
         <v>413</v>
       </c>
-      <c r="E11" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F11" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" t="s">
         <v>236</v>
       </c>
@@ -4444,12 +4508,8 @@
       <c r="D12" t="s">
         <v>414</v>
       </c>
-      <c r="E12" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F12" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" t="s">
         <v>236</v>
       </c>
@@ -4467,12 +4527,8 @@
       <c r="D13" t="s">
         <v>415</v>
       </c>
-      <c r="E13" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F13" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="G13" t="s">
         <v>236</v>
       </c>
@@ -4490,12 +4546,8 @@
       <c r="D14" t="s">
         <v>416</v>
       </c>
-      <c r="E14" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F14" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" t="s">
         <v>236</v>
       </c>
@@ -4513,12 +4565,8 @@
       <c r="D15" t="s">
         <v>417</v>
       </c>
-      <c r="E15" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F15" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="G15" t="s">
         <v>236</v>
       </c>
@@ -4536,12 +4584,8 @@
       <c r="D16" t="s">
         <v>418</v>
       </c>
-      <c r="E16" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F16" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
       <c r="G16" t="s">
         <v>236</v>
       </c>
@@ -4559,12 +4603,8 @@
       <c r="D17" t="s">
         <v>419</v>
       </c>
-      <c r="E17" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F17" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
       <c r="G17" t="s">
         <v>236</v>
       </c>
@@ -4582,12 +4622,8 @@
       <c r="D18" t="s">
         <v>420</v>
       </c>
-      <c r="E18" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F18" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" t="s">
         <v>236</v>
       </c>
@@ -4605,12 +4641,8 @@
       <c r="D19" t="s">
         <v>421</v>
       </c>
-      <c r="E19" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F19" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
       <c r="G19" t="s">
         <v>236</v>
       </c>
@@ -4628,12 +4660,8 @@
       <c r="D20" t="s">
         <v>422</v>
       </c>
-      <c r="E20" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F20" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="G20" t="s">
         <v>236</v>
       </c>
@@ -4651,12 +4679,8 @@
       <c r="D21" t="s">
         <v>423</v>
       </c>
-      <c r="E21" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F21" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
       <c r="G21" t="s">
         <v>236</v>
       </c>
@@ -4674,12 +4698,8 @@
       <c r="D22" t="s">
         <v>424</v>
       </c>
-      <c r="E22" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F22" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" t="s">
         <v>236</v>
       </c>
@@ -4697,12 +4717,8 @@
       <c r="D23" t="s">
         <v>425</v>
       </c>
-      <c r="E23" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F23" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
       <c r="G23" t="s">
         <v>10</v>
       </c>
@@ -4720,12 +4736,8 @@
       <c r="D24" t="s">
         <v>573</v>
       </c>
-      <c r="E24" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F24" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
       <c r="G24" t="s">
         <v>240</v>
       </c>
@@ -4743,12 +4755,8 @@
       <c r="D25" t="s">
         <v>427</v>
       </c>
-      <c r="E25" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F25" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" t="s">
         <v>238</v>
       </c>
@@ -4766,12 +4774,8 @@
       <c r="D26" t="s">
         <v>428</v>
       </c>
-      <c r="E26" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F26" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
       <c r="G26" t="s">
         <v>238</v>
       </c>
@@ -4789,12 +4793,8 @@
       <c r="D27" t="s">
         <v>429</v>
       </c>
-      <c r="E27" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F27" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" t="s">
         <v>238</v>
       </c>
@@ -4812,12 +4812,8 @@
       <c r="D28" t="s">
         <v>430</v>
       </c>
-      <c r="E28" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F28" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" t="s">
         <v>238</v>
       </c>
@@ -4835,12 +4831,8 @@
       <c r="D29" t="s">
         <v>431</v>
       </c>
-      <c r="E29" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F29" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
       <c r="G29" t="s">
         <v>238</v>
       </c>
@@ -4858,12 +4850,8 @@
       <c r="D30" t="s">
         <v>432</v>
       </c>
-      <c r="E30" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F30" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
       <c r="G30" t="s">
         <v>238</v>
       </c>
@@ -4881,12 +4869,8 @@
       <c r="D31" t="s">
         <v>433</v>
       </c>
-      <c r="E31" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F31" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
       <c r="G31" t="s">
         <v>10</v>
       </c>
@@ -4904,12 +4888,8 @@
       <c r="D32" t="s">
         <v>434</v>
       </c>
-      <c r="E32" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F32" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
       <c r="G32" t="s">
         <v>10</v>
       </c>
@@ -4927,12 +4907,8 @@
       <c r="D33" t="s">
         <v>574</v>
       </c>
-      <c r="E33" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F33" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
       <c r="G33" t="s">
         <v>240</v>
       </c>
@@ -4950,12 +4926,8 @@
       <c r="D34" t="s">
         <v>436</v>
       </c>
-      <c r="E34" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F34" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
       <c r="G34" t="s">
         <v>238</v>
       </c>
@@ -4973,12 +4945,8 @@
       <c r="D35" t="s">
         <v>437</v>
       </c>
-      <c r="E35" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F35" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
       <c r="G35" t="s">
         <v>238</v>
       </c>
@@ -4996,12 +4964,8 @@
       <c r="D36" t="s">
         <v>438</v>
       </c>
-      <c r="E36" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F36" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
       <c r="G36" t="s">
         <v>238</v>
       </c>
@@ -5019,12 +4983,8 @@
       <c r="D37" t="s">
         <v>439</v>
       </c>
-      <c r="E37" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F37" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
       <c r="G37" t="s">
         <v>238</v>
       </c>
@@ -5042,12 +5002,8 @@
       <c r="D38" t="s">
         <v>440</v>
       </c>
-      <c r="E38" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F38" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
       <c r="G38" t="s">
         <v>238</v>
       </c>
@@ -5065,12 +5021,8 @@
       <c r="D39" t="s">
         <v>441</v>
       </c>
-      <c r="E39" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F39" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
       <c r="G39" t="s">
         <v>238</v>
       </c>
@@ -5088,12 +5040,8 @@
       <c r="D40" t="s">
         <v>442</v>
       </c>
-      <c r="E40" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F40" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
       <c r="G40" t="s">
         <v>10</v>
       </c>
@@ -5111,12 +5059,8 @@
       <c r="D41" t="s">
         <v>443</v>
       </c>
-      <c r="E41" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F41" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
       <c r="G41" t="s">
         <v>10</v>
       </c>
@@ -5134,12 +5078,8 @@
       <c r="D42" t="s">
         <v>575</v>
       </c>
-      <c r="E42" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F42" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
       <c r="G42" t="s">
         <v>240</v>
       </c>
@@ -5157,12 +5097,8 @@
       <c r="D43" t="s">
         <v>445</v>
       </c>
-      <c r="E43" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F43" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
       <c r="G43" t="s">
         <v>238</v>
       </c>
@@ -5180,12 +5116,8 @@
       <c r="D44" t="s">
         <v>446</v>
       </c>
-      <c r="E44" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F44" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
       <c r="G44" t="s">
         <v>238</v>
       </c>
@@ -5203,12 +5135,8 @@
       <c r="D45" t="s">
         <v>447</v>
       </c>
-      <c r="E45" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F45" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
       <c r="G45" t="s">
         <v>238</v>
       </c>
@@ -5226,12 +5154,8 @@
       <c r="D46" t="s">
         <v>448</v>
       </c>
-      <c r="E46" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F46" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
       <c r="G46" t="s">
         <v>238</v>
       </c>
@@ -5249,12 +5173,8 @@
       <c r="D47" t="s">
         <v>449</v>
       </c>
-      <c r="E47" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F47" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
       <c r="G47" t="s">
         <v>238</v>
       </c>
@@ -5272,12 +5192,8 @@
       <c r="D48" t="s">
         <v>450</v>
       </c>
-      <c r="E48" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F48" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
       <c r="G48" t="s">
         <v>238</v>
       </c>
@@ -5295,12 +5211,8 @@
       <c r="D49" t="s">
         <v>451</v>
       </c>
-      <c r="E49" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F49" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
       <c r="G49" t="s">
         <v>10</v>
       </c>
@@ -5318,12 +5230,8 @@
       <c r="D50" t="s">
         <v>452</v>
       </c>
-      <c r="E50" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F50" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
       <c r="G50" t="s">
         <v>10</v>
       </c>
@@ -5341,12 +5249,8 @@
       <c r="D51" t="s">
         <v>576</v>
       </c>
-      <c r="E51" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F51" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
       <c r="G51" t="s">
         <v>240</v>
       </c>
@@ -5364,12 +5268,8 @@
       <c r="D52" t="s">
         <v>454</v>
       </c>
-      <c r="E52" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F52" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
       <c r="G52" t="s">
         <v>238</v>
       </c>
@@ -5387,12 +5287,8 @@
       <c r="D53" t="s">
         <v>455</v>
       </c>
-      <c r="E53" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F53" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
       <c r="G53" t="s">
         <v>238</v>
       </c>
@@ -5410,12 +5306,8 @@
       <c r="D54" t="s">
         <v>456</v>
       </c>
-      <c r="E54" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F54" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
       <c r="G54" t="s">
         <v>238</v>
       </c>
@@ -5433,12 +5325,8 @@
       <c r="D55" t="s">
         <v>457</v>
       </c>
-      <c r="E55" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F55" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
       <c r="G55" t="s">
         <v>238</v>
       </c>
@@ -5456,12 +5344,8 @@
       <c r="D56" t="s">
         <v>458</v>
       </c>
-      <c r="E56" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F56" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
       <c r="G56" t="s">
         <v>238</v>
       </c>
@@ -5479,12 +5363,8 @@
       <c r="D57" t="s">
         <v>459</v>
       </c>
-      <c r="E57" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F57" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
       <c r="G57" t="s">
         <v>238</v>
       </c>
@@ -5502,12 +5382,8 @@
       <c r="D58" t="s">
         <v>460</v>
       </c>
-      <c r="E58" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F58" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
       <c r="G58" t="s">
         <v>10</v>
       </c>
@@ -5525,12 +5401,8 @@
       <c r="D59" t="s">
         <v>461</v>
       </c>
-      <c r="E59" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F59" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
       <c r="G59" t="s">
         <v>10</v>
       </c>
@@ -5548,12 +5420,8 @@
       <c r="D60" t="s">
         <v>577</v>
       </c>
-      <c r="E60" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F60" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
       <c r="G60" t="s">
         <v>240</v>
       </c>
@@ -5571,12 +5439,8 @@
       <c r="D61" t="s">
         <v>463</v>
       </c>
-      <c r="E61" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F61" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
       <c r="G61" t="s">
         <v>238</v>
       </c>
@@ -5594,12 +5458,8 @@
       <c r="D62" t="s">
         <v>464</v>
       </c>
-      <c r="E62" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F62" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
       <c r="G62" t="s">
         <v>238</v>
       </c>
@@ -5617,12 +5477,8 @@
       <c r="D63" t="s">
         <v>465</v>
       </c>
-      <c r="E63" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F63" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
       <c r="G63" t="s">
         <v>238</v>
       </c>
@@ -5640,12 +5496,8 @@
       <c r="D64" t="s">
         <v>466</v>
       </c>
-      <c r="E64" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F64" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
       <c r="G64" t="s">
         <v>238</v>
       </c>
@@ -5663,12 +5515,8 @@
       <c r="D65" t="s">
         <v>467</v>
       </c>
-      <c r="E65" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F65" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
       <c r="G65" t="s">
         <v>238</v>
       </c>
@@ -5686,12 +5534,8 @@
       <c r="D66" t="s">
         <v>468</v>
       </c>
-      <c r="E66" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F66" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
       <c r="G66" t="s">
         <v>238</v>
       </c>
@@ -5709,12 +5553,8 @@
       <c r="D67" t="s">
         <v>469</v>
       </c>
-      <c r="E67" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F67" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
       <c r="G67" t="s">
         <v>10</v>
       </c>
@@ -5732,12 +5572,8 @@
       <c r="D68" t="s">
         <v>470</v>
       </c>
-      <c r="E68" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F68" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
       <c r="G68" t="s">
         <v>10</v>
       </c>
@@ -5755,12 +5591,8 @@
       <c r="D69" t="s">
         <v>578</v>
       </c>
-      <c r="E69" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F69" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
       <c r="G69" t="s">
         <v>240</v>
       </c>
@@ -5778,12 +5610,8 @@
       <c r="D70" t="s">
         <v>472</v>
       </c>
-      <c r="E70" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F70" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
       <c r="G70" t="s">
         <v>238</v>
       </c>
@@ -5801,12 +5629,8 @@
       <c r="D71" t="s">
         <v>473</v>
       </c>
-      <c r="E71" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F71" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
       <c r="G71" t="s">
         <v>238</v>
       </c>
@@ -5824,12 +5648,8 @@
       <c r="D72" t="s">
         <v>474</v>
       </c>
-      <c r="E72" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F72" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
       <c r="G72" t="s">
         <v>238</v>
       </c>
@@ -5847,12 +5667,8 @@
       <c r="D73" t="s">
         <v>475</v>
       </c>
-      <c r="E73" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F73" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
       <c r="G73" t="s">
         <v>238</v>
       </c>
@@ -5870,12 +5686,8 @@
       <c r="D74" t="s">
         <v>476</v>
       </c>
-      <c r="E74" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F74" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
       <c r="G74" t="s">
         <v>238</v>
       </c>
@@ -5893,12 +5705,8 @@
       <c r="D75" t="s">
         <v>477</v>
       </c>
-      <c r="E75" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F75" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
       <c r="G75" t="s">
         <v>238</v>
       </c>
@@ -5916,12 +5724,8 @@
       <c r="D76" t="s">
         <v>478</v>
       </c>
-      <c r="E76" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F76" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
       <c r="G76" t="s">
         <v>10</v>
       </c>
@@ -5939,12 +5743,8 @@
       <c r="D77" t="s">
         <v>479</v>
       </c>
-      <c r="E77" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F77" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
       <c r="G77" t="s">
         <v>10</v>
       </c>
@@ -5962,12 +5762,8 @@
       <c r="D78" t="s">
         <v>579</v>
       </c>
-      <c r="E78" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F78" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
       <c r="G78" t="s">
         <v>240</v>
       </c>
@@ -5985,12 +5781,8 @@
       <c r="D79" t="s">
         <v>481</v>
       </c>
-      <c r="E79" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F79" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
       <c r="G79" t="s">
         <v>238</v>
       </c>
@@ -6008,12 +5800,8 @@
       <c r="D80" t="s">
         <v>482</v>
       </c>
-      <c r="E80" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F80" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
       <c r="G80" t="s">
         <v>238</v>
       </c>
@@ -6031,12 +5819,8 @@
       <c r="D81" t="s">
         <v>483</v>
       </c>
-      <c r="E81" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F81" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
       <c r="G81" t="s">
         <v>238</v>
       </c>
@@ -6054,12 +5838,8 @@
       <c r="D82" t="s">
         <v>484</v>
       </c>
-      <c r="E82" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F82" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
       <c r="G82" t="s">
         <v>238</v>
       </c>
@@ -6077,12 +5857,8 @@
       <c r="D83" t="s">
         <v>485</v>
       </c>
-      <c r="E83" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F83" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
       <c r="G83" t="s">
         <v>238</v>
       </c>
@@ -6100,12 +5876,8 @@
       <c r="D84" t="s">
         <v>486</v>
       </c>
-      <c r="E84" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F84" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
       <c r="G84" t="s">
         <v>238</v>
       </c>
@@ -6123,12 +5895,8 @@
       <c r="D85" t="s">
         <v>487</v>
       </c>
-      <c r="E85" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F85" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
       <c r="G85" t="s">
         <v>10</v>
       </c>
@@ -6146,12 +5914,8 @@
       <c r="D86" t="s">
         <v>488</v>
       </c>
-      <c r="E86" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F86" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
       <c r="G86" t="s">
         <v>10</v>
       </c>
@@ -6169,12 +5933,8 @@
       <c r="D87" t="s">
         <v>580</v>
       </c>
-      <c r="E87" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F87" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
       <c r="G87" t="s">
         <v>240</v>
       </c>
@@ -6192,12 +5952,8 @@
       <c r="D88" t="s">
         <v>490</v>
       </c>
-      <c r="E88" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F88" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
       <c r="G88" t="s">
         <v>238</v>
       </c>
@@ -6215,12 +5971,8 @@
       <c r="D89" t="s">
         <v>491</v>
       </c>
-      <c r="E89" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F89" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
       <c r="G89" t="s">
         <v>238</v>
       </c>
@@ -6238,12 +5990,8 @@
       <c r="D90" t="s">
         <v>492</v>
       </c>
-      <c r="E90" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F90" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
       <c r="G90" t="s">
         <v>238</v>
       </c>
@@ -6261,12 +6009,8 @@
       <c r="D91" t="s">
         <v>493</v>
       </c>
-      <c r="E91" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F91" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
       <c r="G91" t="s">
         <v>238</v>
       </c>
@@ -6284,12 +6028,8 @@
       <c r="D92" t="s">
         <v>494</v>
       </c>
-      <c r="E92" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F92" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
       <c r="G92" t="s">
         <v>238</v>
       </c>
@@ -6307,12 +6047,8 @@
       <c r="D93" t="s">
         <v>495</v>
       </c>
-      <c r="E93" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F93" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
       <c r="G93" t="s">
         <v>238</v>
       </c>
@@ -6330,12 +6066,8 @@
       <c r="D94" t="s">
         <v>496</v>
       </c>
-      <c r="E94" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F94" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
       <c r="G94" t="s">
         <v>10</v>
       </c>
@@ -6353,12 +6085,8 @@
       <c r="D95" t="s">
         <v>497</v>
       </c>
-      <c r="E95" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F95" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
       <c r="G95" t="s">
         <v>10</v>
       </c>
@@ -6376,12 +6104,8 @@
       <c r="D96" t="s">
         <v>581</v>
       </c>
-      <c r="E96" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F96" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
       <c r="G96" t="s">
         <v>240</v>
       </c>
@@ -6399,12 +6123,8 @@
       <c r="D97" t="s">
         <v>499</v>
       </c>
-      <c r="E97" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F97" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
       <c r="G97" t="s">
         <v>238</v>
       </c>
@@ -6422,12 +6142,8 @@
       <c r="D98" t="s">
         <v>500</v>
       </c>
-      <c r="E98" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F98" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
       <c r="G98" t="s">
         <v>238</v>
       </c>
@@ -6445,12 +6161,8 @@
       <c r="D99" t="s">
         <v>501</v>
       </c>
-      <c r="E99" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F99" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
       <c r="G99" t="s">
         <v>238</v>
       </c>
@@ -6468,12 +6180,8 @@
       <c r="D100" t="s">
         <v>502</v>
       </c>
-      <c r="E100" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F100" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
       <c r="G100" t="s">
         <v>238</v>
       </c>
@@ -6491,12 +6199,8 @@
       <c r="D101" t="s">
         <v>503</v>
       </c>
-      <c r="E101" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F101" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
       <c r="G101" t="s">
         <v>238</v>
       </c>
@@ -6514,12 +6218,8 @@
       <c r="D102" t="s">
         <v>504</v>
       </c>
-      <c r="E102" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F102" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
       <c r="G102" t="s">
         <v>238</v>
       </c>
@@ -6537,12 +6237,8 @@
       <c r="D103" t="s">
         <v>505</v>
       </c>
-      <c r="E103" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F103" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
       <c r="G103" t="s">
         <v>10</v>
       </c>
@@ -6560,12 +6256,8 @@
       <c r="D104" t="s">
         <v>506</v>
       </c>
-      <c r="E104" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F104" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
       <c r="G104" t="s">
         <v>10</v>
       </c>
@@ -6583,12 +6275,8 @@
       <c r="D105" t="s">
         <v>582</v>
       </c>
-      <c r="E105" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F105" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
       <c r="G105" t="s">
         <v>240</v>
       </c>
@@ -6606,12 +6294,8 @@
       <c r="D106" t="s">
         <v>508</v>
       </c>
-      <c r="E106" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F106" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
       <c r="G106" t="s">
         <v>238</v>
       </c>
@@ -6629,12 +6313,8 @@
       <c r="D107" t="s">
         <v>509</v>
       </c>
-      <c r="E107" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F107" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
       <c r="G107" t="s">
         <v>238</v>
       </c>
@@ -6652,12 +6332,8 @@
       <c r="D108" t="s">
         <v>510</v>
       </c>
-      <c r="E108" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F108" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
       <c r="G108" t="s">
         <v>238</v>
       </c>
@@ -6675,12 +6351,8 @@
       <c r="D109" t="s">
         <v>511</v>
       </c>
-      <c r="E109" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F109" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
       <c r="G109" t="s">
         <v>238</v>
       </c>
@@ -6698,12 +6370,8 @@
       <c r="D110" t="s">
         <v>512</v>
       </c>
-      <c r="E110" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F110" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
       <c r="G110" t="s">
         <v>238</v>
       </c>
@@ -6721,12 +6389,8 @@
       <c r="D111" t="s">
         <v>513</v>
       </c>
-      <c r="E111" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F111" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
       <c r="G111" t="s">
         <v>238</v>
       </c>
@@ -6744,12 +6408,8 @@
       <c r="D112" t="s">
         <v>514</v>
       </c>
-      <c r="E112" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F112" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
       <c r="G112" t="s">
         <v>10</v>
       </c>
@@ -6767,12 +6427,8 @@
       <c r="D113" t="s">
         <v>515</v>
       </c>
-      <c r="E113" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F113" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
       <c r="G113" t="s">
         <v>10</v>
       </c>
@@ -6790,12 +6446,8 @@
       <c r="D114" t="s">
         <v>583</v>
       </c>
-      <c r="E114" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F114" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
       <c r="G114" t="s">
         <v>240</v>
       </c>
@@ -6813,12 +6465,8 @@
       <c r="D115" t="s">
         <v>517</v>
       </c>
-      <c r="E115" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F115" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
       <c r="G115" t="s">
         <v>238</v>
       </c>
@@ -6836,12 +6484,8 @@
       <c r="D116" t="s">
         <v>518</v>
       </c>
-      <c r="E116" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F116" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
       <c r="G116" t="s">
         <v>238</v>
       </c>
@@ -6859,12 +6503,8 @@
       <c r="D117" t="s">
         <v>519</v>
       </c>
-      <c r="E117" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F117" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
       <c r="G117" t="s">
         <v>238</v>
       </c>
@@ -6882,12 +6522,8 @@
       <c r="D118" t="s">
         <v>520</v>
       </c>
-      <c r="E118" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F118" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
       <c r="G118" t="s">
         <v>238</v>
       </c>
@@ -6905,12 +6541,8 @@
       <c r="D119" t="s">
         <v>521</v>
       </c>
-      <c r="E119" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F119" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
       <c r="G119" t="s">
         <v>238</v>
       </c>
@@ -6928,12 +6560,8 @@
       <c r="D120" t="s">
         <v>522</v>
       </c>
-      <c r="E120" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F120" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
       <c r="G120" t="s">
         <v>238</v>
       </c>
@@ -6951,12 +6579,8 @@
       <c r="D121" t="s">
         <v>523</v>
       </c>
-      <c r="E121" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F121" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
       <c r="G121" t="s">
         <v>10</v>
       </c>
@@ -6974,12 +6598,8 @@
       <c r="D122" t="s">
         <v>524</v>
       </c>
-      <c r="E122" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F122" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
       <c r="G122" t="s">
         <v>10</v>
       </c>
@@ -6997,12 +6617,8 @@
       <c r="D123" t="s">
         <v>584</v>
       </c>
-      <c r="E123" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F123" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
       <c r="G123" t="s">
         <v>240</v>
       </c>
@@ -7020,12 +6636,8 @@
       <c r="D124" t="s">
         <v>526</v>
       </c>
-      <c r="E124" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F124" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
       <c r="G124" t="s">
         <v>238</v>
       </c>
@@ -7043,12 +6655,8 @@
       <c r="D125" t="s">
         <v>527</v>
       </c>
-      <c r="E125" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F125" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
       <c r="G125" t="s">
         <v>238</v>
       </c>
@@ -7066,12 +6674,8 @@
       <c r="D126" t="s">
         <v>528</v>
       </c>
-      <c r="E126" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F126" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
       <c r="G126" t="s">
         <v>238</v>
       </c>
@@ -7089,12 +6693,8 @@
       <c r="D127" t="s">
         <v>529</v>
       </c>
-      <c r="E127" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F127" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
       <c r="G127" t="s">
         <v>238</v>
       </c>
@@ -7112,12 +6712,8 @@
       <c r="D128" t="s">
         <v>530</v>
       </c>
-      <c r="E128" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F128" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
       <c r="G128" t="s">
         <v>238</v>
       </c>
@@ -7135,12 +6731,8 @@
       <c r="D129" t="s">
         <v>531</v>
       </c>
-      <c r="E129" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F129" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
       <c r="G129" t="s">
         <v>238</v>
       </c>
@@ -7158,12 +6750,8 @@
       <c r="D130" t="s">
         <v>532</v>
       </c>
-      <c r="E130" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F130" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
       <c r="G130" t="s">
         <v>10</v>
       </c>
@@ -7181,12 +6769,8 @@
       <c r="D131" t="s">
         <v>533</v>
       </c>
-      <c r="E131" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F131" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
       <c r="G131" t="s">
         <v>10</v>
       </c>
@@ -7204,12 +6788,8 @@
       <c r="D132" t="s">
         <v>585</v>
       </c>
-      <c r="E132" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F132" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
       <c r="G132" t="s">
         <v>240</v>
       </c>
@@ -7227,12 +6807,8 @@
       <c r="D133" t="s">
         <v>535</v>
       </c>
-      <c r="E133" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F133" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
       <c r="G133" t="s">
         <v>238</v>
       </c>
@@ -7250,12 +6826,8 @@
       <c r="D134" t="s">
         <v>536</v>
       </c>
-      <c r="E134" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F134" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
       <c r="G134" t="s">
         <v>238</v>
       </c>
@@ -7273,12 +6845,8 @@
       <c r="D135" t="s">
         <v>537</v>
       </c>
-      <c r="E135" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F135" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
       <c r="G135" t="s">
         <v>238</v>
       </c>
@@ -7296,12 +6864,8 @@
       <c r="D136" t="s">
         <v>538</v>
       </c>
-      <c r="E136" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F136" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
       <c r="G136" t="s">
         <v>238</v>
       </c>
@@ -7319,12 +6883,8 @@
       <c r="D137" t="s">
         <v>539</v>
       </c>
-      <c r="E137" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F137" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
       <c r="G137" t="s">
         <v>238</v>
       </c>
@@ -7342,12 +6902,8 @@
       <c r="D138" t="s">
         <v>540</v>
       </c>
-      <c r="E138" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F138" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
       <c r="G138" t="s">
         <v>238</v>
       </c>
@@ -7365,12 +6921,8 @@
       <c r="D139" t="s">
         <v>541</v>
       </c>
-      <c r="E139" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F139" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
       <c r="G139" t="s">
         <v>10</v>
       </c>
@@ -7388,12 +6940,8 @@
       <c r="D140" t="s">
         <v>542</v>
       </c>
-      <c r="E140" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F140" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
       <c r="G140" t="s">
         <v>10</v>
       </c>
@@ -7411,12 +6959,8 @@
       <c r="D141" t="s">
         <v>586</v>
       </c>
-      <c r="E141" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F141" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
       <c r="G141" t="s">
         <v>240</v>
       </c>
@@ -7434,12 +6978,8 @@
       <c r="D142" t="s">
         <v>544</v>
       </c>
-      <c r="E142" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F142" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
       <c r="G142" t="s">
         <v>238</v>
       </c>
@@ -7457,12 +6997,8 @@
       <c r="D143" t="s">
         <v>545</v>
       </c>
-      <c r="E143" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F143" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
       <c r="G143" t="s">
         <v>238</v>
       </c>
@@ -7480,12 +7016,8 @@
       <c r="D144" t="s">
         <v>546</v>
       </c>
-      <c r="E144" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F144" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
       <c r="G144" t="s">
         <v>238</v>
       </c>
@@ -7503,12 +7035,8 @@
       <c r="D145" t="s">
         <v>547</v>
       </c>
-      <c r="E145" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F145" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
       <c r="G145" t="s">
         <v>238</v>
       </c>
@@ -7526,12 +7054,8 @@
       <c r="D146" t="s">
         <v>548</v>
       </c>
-      <c r="E146" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F146" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
       <c r="G146" t="s">
         <v>238</v>
       </c>
@@ -7549,12 +7073,8 @@
       <c r="D147" t="s">
         <v>549</v>
       </c>
-      <c r="E147" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F147" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
       <c r="G147" t="s">
         <v>238</v>
       </c>
@@ -7572,12 +7092,8 @@
       <c r="D148" t="s">
         <v>550</v>
       </c>
-      <c r="E148" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F148" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
       <c r="G148" t="s">
         <v>10</v>
       </c>
@@ -7595,12 +7111,8 @@
       <c r="D149" t="s">
         <v>551</v>
       </c>
-      <c r="E149" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F149" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
       <c r="G149" t="s">
         <v>10</v>
       </c>
@@ -7618,12 +7130,8 @@
       <c r="D150" t="s">
         <v>587</v>
       </c>
-      <c r="E150" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F150" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
       <c r="G150" t="s">
         <v>240</v>
       </c>
@@ -7641,12 +7149,8 @@
       <c r="D151" t="s">
         <v>553</v>
       </c>
-      <c r="E151" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F151" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
       <c r="G151" t="s">
         <v>238</v>
       </c>
@@ -7664,12 +7168,8 @@
       <c r="D152" t="s">
         <v>554</v>
       </c>
-      <c r="E152" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F152" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
       <c r="G152" t="s">
         <v>238</v>
       </c>
@@ -7687,12 +7187,8 @@
       <c r="D153" t="s">
         <v>555</v>
       </c>
-      <c r="E153" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F153" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
       <c r="G153" t="s">
         <v>238</v>
       </c>
@@ -7710,12 +7206,8 @@
       <c r="D154" t="s">
         <v>556</v>
       </c>
-      <c r="E154" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F154" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
       <c r="G154" t="s">
         <v>238</v>
       </c>
@@ -7733,12 +7225,8 @@
       <c r="D155" t="s">
         <v>557</v>
       </c>
-      <c r="E155" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F155" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
       <c r="G155" t="s">
         <v>238</v>
       </c>
@@ -7756,12 +7244,8 @@
       <c r="D156" t="s">
         <v>558</v>
       </c>
-      <c r="E156" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F156" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
       <c r="G156" t="s">
         <v>238</v>
       </c>
@@ -7779,12 +7263,8 @@
       <c r="D157" t="s">
         <v>559</v>
       </c>
-      <c r="E157" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F157" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
       <c r="G157" t="s">
         <v>10</v>
       </c>
@@ -7802,12 +7282,8 @@
       <c r="D158" t="s">
         <v>560</v>
       </c>
-      <c r="E158" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F158" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
       <c r="G158" t="s">
         <v>10</v>
       </c>
@@ -7825,12 +7301,8 @@
       <c r="D159" t="s">
         <v>588</v>
       </c>
-      <c r="E159" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F159" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
       <c r="G159" t="s">
         <v>240</v>
       </c>
@@ -7848,12 +7320,8 @@
       <c r="D160" t="s">
         <v>562</v>
       </c>
-      <c r="E160" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F160" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
       <c r="G160" t="s">
         <v>238</v>
       </c>
@@ -7871,12 +7339,8 @@
       <c r="D161" t="s">
         <v>563</v>
       </c>
-      <c r="E161" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F161" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
       <c r="G161" t="s">
         <v>238</v>
       </c>
@@ -7894,12 +7358,8 @@
       <c r="D162" t="s">
         <v>564</v>
       </c>
-      <c r="E162" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F162" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
       <c r="G162" t="s">
         <v>238</v>
       </c>
@@ -7917,12 +7377,8 @@
       <c r="D163" t="s">
         <v>565</v>
       </c>
-      <c r="E163" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F163" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
       <c r="G163" t="s">
         <v>238</v>
       </c>
@@ -7940,12 +7396,8 @@
       <c r="D164" t="s">
         <v>566</v>
       </c>
-      <c r="E164" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F164" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
       <c r="G164" t="s">
         <v>238</v>
       </c>
@@ -7963,12 +7415,8 @@
       <c r="D165" t="s">
         <v>567</v>
       </c>
-      <c r="E165" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F165" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
       <c r="G165" t="s">
         <v>238</v>
       </c>
@@ -7986,12 +7434,8 @@
       <c r="D166" t="s">
         <v>568</v>
       </c>
-      <c r="E166" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F166" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
       <c r="G166" t="s">
         <v>10</v>
       </c>
@@ -8009,12 +7453,8 @@
       <c r="D167" t="s">
         <v>569</v>
       </c>
-      <c r="E167" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F167" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
       <c r="G167" t="s">
         <v>10</v>
       </c>
@@ -8032,12 +7472,8 @@
       <c r="D168" t="s">
         <v>570</v>
       </c>
-      <c r="E168" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F168" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
       <c r="G168" t="s">
         <v>11</v>
       </c>
@@ -8055,12 +7491,8 @@
       <c r="D169" t="s">
         <v>571</v>
       </c>
-      <c r="E169" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F169" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
       <c r="G169" t="s">
         <v>13</v>
       </c>
@@ -8078,12 +7510,8 @@
       <c r="D170" t="s">
         <v>572</v>
       </c>
-      <c r="E170" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F170" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
       <c r="G170" t="s">
         <v>14</v>
       </c>
@@ -8101,12 +7529,8 @@
       <c r="D171" t="s">
         <v>426</v>
       </c>
-      <c r="E171" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F171" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
       <c r="G171" t="s">
         <v>387</v>
       </c>
@@ -8124,12 +7548,8 @@
       <c r="D172" t="s">
         <v>435</v>
       </c>
-      <c r="E172" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F172" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
       <c r="G172" t="s">
         <v>387</v>
       </c>
@@ -8147,12 +7567,8 @@
       <c r="D173" t="s">
         <v>444</v>
       </c>
-      <c r="E173" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F173" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
       <c r="G173" t="s">
         <v>387</v>
       </c>
@@ -8170,12 +7586,8 @@
       <c r="D174" t="s">
         <v>453</v>
       </c>
-      <c r="E174" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F174" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E174" s="2"/>
+      <c r="F174" s="2"/>
       <c r="G174" t="s">
         <v>387</v>
       </c>
@@ -8193,12 +7605,8 @@
       <c r="D175" t="s">
         <v>462</v>
       </c>
-      <c r="E175" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F175" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
       <c r="G175" t="s">
         <v>387</v>
       </c>
@@ -8216,12 +7624,8 @@
       <c r="D176" t="s">
         <v>471</v>
       </c>
-      <c r="E176" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F176" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
       <c r="G176" t="s">
         <v>387</v>
       </c>
@@ -8239,12 +7643,8 @@
       <c r="D177" t="s">
         <v>480</v>
       </c>
-      <c r="E177" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F177" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E177" s="2"/>
+      <c r="F177" s="2"/>
       <c r="G177" t="s">
         <v>387</v>
       </c>
@@ -8262,12 +7662,8 @@
       <c r="D178" t="s">
         <v>489</v>
       </c>
-      <c r="E178" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F178" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
       <c r="G178" t="s">
         <v>387</v>
       </c>
@@ -8285,12 +7681,8 @@
       <c r="D179" t="s">
         <v>498</v>
       </c>
-      <c r="E179" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F179" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
       <c r="G179" t="s">
         <v>387</v>
       </c>
@@ -8308,12 +7700,8 @@
       <c r="D180" t="s">
         <v>507</v>
       </c>
-      <c r="E180" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F180" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E180" s="2"/>
+      <c r="F180" s="2"/>
       <c r="G180" t="s">
         <v>387</v>
       </c>
@@ -8331,12 +7719,8 @@
       <c r="D181" t="s">
         <v>516</v>
       </c>
-      <c r="E181" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F181" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
       <c r="G181" t="s">
         <v>387</v>
       </c>
@@ -8354,12 +7738,8 @@
       <c r="D182" t="s">
         <v>525</v>
       </c>
-      <c r="E182" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F182" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
       <c r="G182" t="s">
         <v>387</v>
       </c>
@@ -8377,12 +7757,8 @@
       <c r="D183" t="s">
         <v>534</v>
       </c>
-      <c r="E183" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F183" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E183" s="2"/>
+      <c r="F183" s="2"/>
       <c r="G183" t="s">
         <v>387</v>
       </c>
@@ -8400,12 +7776,8 @@
       <c r="D184" t="s">
         <v>543</v>
       </c>
-      <c r="E184" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F184" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E184" s="2"/>
+      <c r="F184" s="2"/>
       <c r="G184" t="s">
         <v>387</v>
       </c>
@@ -8423,12 +7795,8 @@
       <c r="D185" t="s">
         <v>552</v>
       </c>
-      <c r="E185" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F185" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
       <c r="G185" t="s">
         <v>387</v>
       </c>
@@ -8446,12 +7814,8 @@
       <c r="D186" t="s">
         <v>561</v>
       </c>
-      <c r="E186" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F186" s="2">
-        <v>54798</v>
-      </c>
+      <c r="E186" s="2"/>
+      <c r="F186" s="2"/>
       <c r="G186" t="s">
         <v>387</v>
       </c>

</xml_diff>